<commit_message>
Bulma and others changed/Improved
</commit_message>
<xml_diff>
--- a/CSS Frameworks (Bulma and Tailwind) Cheatsheet.xlsx
+++ b/CSS Frameworks (Bulma and Tailwind) Cheatsheet.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\conor\My Drive\Cheatsheet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\conor\My Drive\Cheatsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D0D6426-B033-45FD-A2F0-4715C8C39937}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F30C8EF0-6799-4017-80A8-EF9A0FE56817}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28695" yWindow="6015" windowWidth="14610" windowHeight="15585" xr2:uid="{6EA60963-E8CF-4A17-BC36-F719854BE9A4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{6EA60963-E8CF-4A17-BC36-F719854BE9A4}"/>
   </bookViews>
   <sheets>
-    <sheet name="Bulma" sheetId="1" r:id="rId1"/>
+    <sheet name="Bulma Basics" sheetId="1" r:id="rId1"/>
+    <sheet name="Bulma Class Addons More Detail" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -78,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="67">
   <si>
     <t>Concept</t>
   </si>
@@ -126,11 +127,6 @@
         &lt;/div&gt;
     &lt;/div&gt;
 &lt;/section&gt;</t>
-  </si>
-  <si>
-    <t>The hero section of a website is the main part of the website that is loaded when you go onto a webpage. E.g. the Nissan website, the body usually takes up most of the top of the page when you load it, but it also doesn't the toolbox at the top.
-To create a hero, you first start with the &lt;section&gt; tab, then add class="hero". After this, you create a div between with class="hero-body", and a div below that called using class="container"
-After this you can then add everything within the tagged bit within the container. The hero is able to encompass almost anything else, including "navbar"s and other things.</t>
   </si>
   <si>
     <r>
@@ -259,10 +255,6 @@
 &lt;/section&gt;</t>
   </si>
   <si>
-    <t>The columns are contained within a container, which itself is contained with a section. Underneath, you create a div with class="columns", then within this you can create individual columns with class="column". It automatically changes the page based on how many columns you have, and adjust accordingly.
-It's something to look out for: much of what is made is with a div class="container", and then these things can be within &lt;section&gt; tags. Unless it's a specific type of section, then the section class is just "section"</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">We can force the width of each individual column now matter how many are on a single line with the </t>
     </r>
@@ -317,9 +309,6 @@
   <si>
     <t>Notification:
 &lt;div class="notification"&gt; … &lt;/div&gt;</t>
-  </si>
-  <si>
-    <t>Notification envelops a portion of the code into a notification-type area. It's a small thing to add, but it can make certain aspects of our website more interesting. Notifications are very similar to cards (shown later), but cards very often are able to hold a lot more information.</t>
   </si>
   <si>
     <t>Editing text</t>
@@ -572,9 +561,6 @@
     <t>&lt;div class="content"&gt;
   &lt;h1&gt;…&lt;/h1&gt;
 &lt;/div&gt;</t>
-  </si>
-  <si>
-    <t>The content class in Bulma is perhaps the class that is the most used out of all bulma classes. It basically makes the process of including text content a hell of a lot easier. All text, h1, h2, p, etc, ends up being included within these sections, in a very neatly and organised fashion.</t>
   </si>
   <si>
     <t>is-small/is-medium/is-large (all to change the size of text in the contents section)</t>
@@ -629,10 +615,6 @@
                 &lt;/div&gt;</t>
   </si>
   <si>
-    <t>The navbar allows for you to have a navigation bar at the top of your image. You include an item with the class of navbar, and you then include a container, then navbar-items underneath, which within them are usually just text, or links.
-The method I prefer for including navbar-item (s) within a document is to include them within a column layout, and within a hero, and hero-head section. We go down the layers, and then within this, we include p tags to include our information in.</t>
-  </si>
-  <si>
     <t>IF we wanted to include an image within a navbar-item, the best way to go about this is to insert it within a figure tag, and write it like this:
 &lt;figure class="navbar-item image"&gt;
   &lt;img src="image.png"
@@ -862,6 +844,748 @@
         <scheme val="minor"/>
       </rPr>
       <t>make buttons round</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>The hero section isn't contained within anything else. It is usually the first layer. After that, hero-head, hero-body, and hero-footer are contained within hero. Within these you can add columns and containers.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+The hero section of a website is the main part of the website that is loaded when you go onto a webpage. E.g. the Nissan website, the body usually takes up most of the top of the page when you load it, but it also doesn't the toolbox at the top.
+To create a hero, you first start with the &lt;section&gt; tab, then add class="hero". After this, you create a div between with class="hero-body", and a div below that called using class="container"
+After this you can then add everything within the tagged bit within the container. The hero is able to encompass almost anything else, including "navbar"s and other things.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Columns should be contained within either one of the hero sections, or within a container, which itself is contained within an ordinary section of class section.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+The columns are contained within a container, which itself is contained with a section. Underneath, you create a div with class="columns", then within this you can create individual columns with class="column". It automatically changes the page based on how many columns you have, and adjust accordingly.
+It's something to look out for: much of what is made is with a div class="container", and then these things can be within &lt;section&gt; tags. Unless it's a specific type of section, then the section class is just "section"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Notifications are best contained within a column (if you are going to have notifications scroll across a single page), or at least within a container.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Notification envelops a portion of the code into a notification-type area. It's a small thing to add, but it can make certain aspects of our website more interesting. Notifications are very similar to cards (shown later), but cards very often are able to hold a lot more information.</t>
+    </r>
+  </si>
+  <si>
+    <t>Hardly used, so cba to go any further with them.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Content class must be within a container, or within a hero-element section</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+The content class in Bulma is perhaps the class that is the most used out of all bulma classes. It basically makes the process of including text content a hell of a lot easier. All text, h1, h2, p, etc, ends up being included within these sections, in a very neatly and organised fashion.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Navbar-item are best contained within individual columns.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+The navbar allows for you to have a navigation bar at the top of your image. You include an item with the class of navbar, and you then include a container, then navbar-items underneath, which within them are usually just text, or links.
+The method I prefer for including navbar-item (s) within a document is to include them within a column layout, and within a hero, and hero-head section. We go down the layers, and then within this, we include p tags to include our information in.</t>
+    </r>
+  </si>
+  <si>
+    <t>If you have multiple navbar-item elements that you're trying to add to hero-head and want to style them well, just use this within the columns:
+Left column: &lt;div class="column" style="justify-content: left; display: flex;"&gt;
+Centre column: &lt;div class="column" style="justify-content: center; display: flex;"&gt;
+Right column: &lt;div class="column" style="justify-content: right; display: flex;"&gt;
+It just makes it look really nice, trust me bro.</t>
+  </si>
+  <si>
+    <t>Text elements</t>
+  </si>
+  <si>
+    <t>navbar-item</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>is-inline</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - It will behave as an inline-block element, allowing it to be displayed inline with other elements in the navbar while also retaining its block-level properties such as padding and margins.</t>
+    </r>
+  </si>
+  <si>
+    <t>section</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">The is-multiline class is quite nice, but it's even nicer if you include this code within a .css file if you haven't defined the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">is-half, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>etc:
+@media screen and (max-width: 768px) {
+    .columns.is-multiline {
+        .column {
+            /* Change 6 to the desired number of columns per row for smaller screens */
+            flex: 1 0 calc(100% / 6);
+        }
+    }
+}
+This piece of code changes the number of items per row depending on what the width of the screen is (e.g. on mobile.). If you want additional options, you can just change the max-width variable, and then change the division to a smaller number.</t>
+    </r>
+  </si>
+  <si>
+    <t>Image</t>
+  </si>
+  <si>
+    <t>If you're placing an image "the bulma way", you're very often going to be writing it within a column, and writing it like this:
+ &lt;div class="column"&gt;
+  &lt;figure class="image"&gt;
+    &lt;img alt="JavaScript" style="height: 64px;"
+      src="https://cdn.worldvectorlogo.com/logos/logo-javascript.svg" /&gt;
+  &lt;/figure&gt;
+&lt;/div&gt;
+With the image within a figure, with class="image"</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>has-text-white</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - Changes text to the colour white. Can also do </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>black, light, primary, info</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, and others.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>has-text-centered</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - Centres the within the container.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">is-size-5 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">- Forces the text to be of size 5 (arbitrary size). If you want to specify different sizes for desktop and mobile, you can do </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">is-size-5-desktop </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">and </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">is-size-6-mobile </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">respectively
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">title - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Changes the styling slightly so that it looks more like title text. Can also do </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>subtitle</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, or others within the different tags</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">has-background-light </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>- Changes the background of the entire section to a particular colour/image. Although this is included within section, in reality it can be added in any other section (e.g. container/notification/card/etc)</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+id-paddingless </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>- Gets rid of all padding between separate elements (in this instance, containers) so that items are more tightly squeezed together</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+is-mobile -</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Enforces a horizontal layout for columns (just always a good thing to add to column classes)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">is-halfheight </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>- Makes the entire hero section half the height of the browser</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Others exists also, and specify different width percentages/proportions</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>is-64x64</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - We can specify the size of the image after we asign the image for certain things. Other options include </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>is-32x32, is-128x128</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. However I've always found that specifying the height in the style section to be more reliable overall.</t>
+    </r>
+  </si>
+  <si>
+    <t>Columns and column classes</t>
+  </si>
+  <si>
+    <t>Hero classes</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">is-marginless </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>- Removes all margins from an element. Sometimes nice to test out the difference between this class in and out</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+heading - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Adds a heading text style to the words. Quite nice for, would you guess it, headings</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+has-text-weight-bold</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - Forces the text to be slightly bold. Alternatives include </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">light, medium, semibold </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">and </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">normal
+is-half </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>- Makes each column take up half the size of the container</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+is-multiline</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - Forces the columns to become multiple lines if things extend beyond the original point. For example, if you have more than two columns and each column has </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>is-half</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, then this class code would automatically push it back underneath.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+is-centered </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>- Centers the columns that you have. If you only have one column, and you've defined a width, then it will center this</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+tile </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>- Within an individual column, before we specify whether we've got a notification/card/etc, we can add tile to the column level. Helpful for arranging content in a grid-like format</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Hard to describe in words, but you've just got to try it</t>
     </r>
   </si>
 </sst>
@@ -933,7 +1657,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -944,11 +1668,75 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="17">
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -1107,15 +1895,27 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E7CE86FC-41ED-4CC0-88F6-21E624060BA1}" name="Table12" displayName="Table12" ref="A1:F13" totalsRowShown="0" headerRowDxfId="9" dataDxfId="7" headerRowBorderDxfId="8" tableBorderDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E7CE86FC-41ED-4CC0-88F6-21E624060BA1}" name="Table12" displayName="Table12" ref="A1:F13" totalsRowShown="0" headerRowDxfId="16" dataDxfId="14" headerRowBorderDxfId="15" tableBorderDxfId="13">
   <autoFilter ref="A1:F13" xr:uid="{E7CE86FC-41ED-4CC0-88F6-21E624060BA1}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{F46920EF-A77D-4D33-90D4-090F93169153}" name="Concept" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{3552D3D7-D45D-46D8-B1A6-926A184395FF}" name="Code" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{2F139388-F80F-4745-BF23-028C637B0A8B}" name="Explained" dataDxfId="3"/>
-    <tableColumn id="7" xr3:uid="{A5181729-E86D-4094-8AF8-397622120A71}" name="Class addons" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{FD0E36D0-D7FC-46F4-AC27-0F23150D4890}" name="Notes" dataDxfId="1"/>
-    <tableColumn id="5" xr3:uid="{56B9D781-3D61-4B8A-AB17-CFFF484AE7F0}" name="Images" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{F46920EF-A77D-4D33-90D4-090F93169153}" name="Concept" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{3552D3D7-D45D-46D8-B1A6-926A184395FF}" name="Code" dataDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{2F139388-F80F-4745-BF23-028C637B0A8B}" name="Explained" dataDxfId="10"/>
+    <tableColumn id="7" xr3:uid="{A5181729-E86D-4094-8AF8-397622120A71}" name="Class addons" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{FD0E36D0-D7FC-46F4-AC27-0F23150D4890}" name="Notes" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{56B9D781-3D61-4B8A-AB17-CFFF484AE7F0}" name="Images" dataDxfId="7"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0F242125-CC3C-4DA6-80FC-4AB6BF881EDF}" name="Table2" displayName="Table2" ref="A1:C7" totalsRowShown="0" headerRowDxfId="2" dataDxfId="1" headerRowBorderDxfId="5" tableBorderDxfId="6">
+  <autoFilter ref="A1:C7" xr:uid="{0F242125-CC3C-4DA6-80FC-4AB6BF881EDF}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{FA01D4D5-0EB3-4BFE-9166-B54519DB94BB}" name="Concept" dataDxfId="0"/>
+    <tableColumn id="4" xr3:uid="{638DEB31-B43F-422B-AF89-C1CBBED4CBB9}" name="Class addons" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{A0FD955E-F2F9-4AF6-AECA-8C4BAABAF104}" name="Notes" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1420,8 +2220,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15A30FB2-92F8-406F-BD78-8EFE04E51E93}">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B8" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1477,13 +2277,13 @@
         <v>11</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>13</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>14</v>
       </c>
       <c r="F3" s="2" t="e" vm="1">
         <v>#VALUE!</v>
@@ -1491,27 +2291,27 @@
     </row>
     <row r="4" spans="1:6" ht="225" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="C4" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="2" t="s">
+    </row>
+    <row r="5" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="B5" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>20</v>
-      </c>
       <c r="C5" s="2" t="s">
-        <v>21</v>
+        <v>48</v>
       </c>
       <c r="F5" s="2" t="e" vm="2">
         <v>#VALUE!</v>
@@ -1519,55 +2319,58 @@
     </row>
     <row r="6" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="E6" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="210" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="E8" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="180" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="B9" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="C9" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E8" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="195" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>35</v>
+      <c r="E9" s="2" t="s">
+        <v>49</v>
       </c>
       <c r="F9" s="2" t="e" vm="3">
         <v>#VALUE!</v>
@@ -1575,52 +2378,144 @@
     </row>
     <row r="10" spans="1:6" ht="195" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>36</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="300" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="270" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>47</v>
+        <v>42</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1AA980B-F412-47A9-8AD5-28D23431EA09}">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25.85546875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="79.28515625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="83.140625" style="2" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="225" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="120" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="105" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="105" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="150" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>